<commit_message>
QUBES Code First commit
</commit_message>
<xml_diff>
--- a/src/main/resources/Inputdata/TestData.xlsx
+++ b/src/main/resources/Inputdata/TestData.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="146">
   <si>
     <t xml:space="preserve">Contact Number Land Line   </t>
   </si>
@@ -345,6 +345,132 @@
   </si>
   <si>
     <t>WPL031047</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220097</t>
+  </si>
+  <si>
+    <t>WPL031048</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220098</t>
+  </si>
+  <si>
+    <t>WPL031049</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220099</t>
+  </si>
+  <si>
+    <t>WPL031050</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220100</t>
+  </si>
+  <si>
+    <t>WPL031051</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220101</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220102</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220103</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220104</t>
+  </si>
+  <si>
+    <t>WPL031055</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220105</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220106</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220107</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220108</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220109</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220110</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220111</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220112</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220113</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220114</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220115</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220116</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220117</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220118</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220119</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220120</t>
+  </si>
+  <si>
+    <t>WPL031070</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220121</t>
+  </si>
+  <si>
+    <t>WPL031071</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220122</t>
+  </si>
+  <si>
+    <t>WPL031072</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220123</t>
+  </si>
+  <si>
+    <t>WPL031073</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220124</t>
+  </si>
+  <si>
+    <t>WPL031074</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220125</t>
+  </si>
+  <si>
+    <t>WPL031075</t>
+  </si>
+  <si>
+    <t>Var1-VS1P320220126</t>
+  </si>
+  <si>
+    <t>WPL031076</t>
   </si>
 </sst>
 </file>
@@ -1017,12 +1143,12 @@
     </row>
     <row r="5">
       <c r="C5" t="s">
-        <v>102</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" t="s">
-        <v>103</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>